<commit_message>
dangtq thêm bb hop ngày 31
</commit_message>
<xml_diff>
--- a/Analysis/Money.xlsx
+++ b/Analysis/Money.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E41E7C1-FC55-48D8-8E5E-39FFAE1C8FC7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B4251F-791E-494A-B04E-3A730574F407}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +24,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tác giả</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{E4ECA354-1215-4257-B82D-03FB47F6265A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tác giả:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tạm ứng lần 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{CEBD0644-2D5B-4FB3-A9F3-B76D46231939}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tác giả:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tiền thiết kế gửi a học</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ĐángTQ</t>
   </si>
@@ -45,7 +103,13 @@
     <t>Ngày</t>
   </si>
   <si>
-    <t>Trả lần 1</t>
+    <t>Tổng chi</t>
+  </si>
+  <si>
+    <t>Tổng thu</t>
+  </si>
+  <si>
+    <t>Còn lại</t>
   </si>
 </sst>
 </file>
@@ -54,9 +118,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +134,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,12 +187,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -396,11 +473,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,13 +497,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <f xml:space="preserve"> SUM(B6,B8,C8,C7,C6,D6)</f>
-        <v>15500000</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -456,16 +527,16 @@
       <c r="D6" s="4">
         <v>3000000</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="4">
         <v>3500000</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -477,68 +548,70 @@
       <c r="C8" s="4">
         <v>3000000</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4">
+        <v>1500000</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17" s="6">
         <f>SUM(B6:B16)</f>
@@ -546,7 +619,7 @@
       </c>
       <c r="C17" s="6">
         <f>SUM(C6:C16)</f>
-        <v>8000000</v>
+        <v>9500000</v>
       </c>
       <c r="D17" s="6">
         <f>SUM(D6:D16)</f>
@@ -554,10 +627,34 @@
       </c>
       <c r="E17" s="6">
         <f>SUM(B17:D17)</f>
-        <v>15500000</v>
+        <v>17000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>66000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
+        <f>E18-E17</f>
+        <v>49000000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>